<commit_message>
cleaned up some things and added a rescue to the excel save
</commit_message>
<xml_diff>
--- a/simple.xlsx
+++ b/simple.xlsx
@@ -152,13 +152,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>21</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1" formatCode="General">
-                  <c:v>11</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2" formatCode="General">
-                  <c:v>17</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -247,7 +247,7 @@
         </is>
       </c>
       <c r="B2" s="0" t="n">
-        <v>21</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3">
@@ -257,7 +257,7 @@
         </is>
       </c>
       <c r="B3" s="0" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
@@ -267,7 +267,7 @@
         </is>
       </c>
       <c r="B4" s="0" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>